<commit_message>
Fix organization name typo: Tirvest -> Trivest Advisors (total 19 users)
</commit_message>
<xml_diff>
--- a/df_users.xlsx
+++ b/df_users.xlsx
@@ -1914,7 +1914,7 @@
       <c r="B61" t="inlineStr"/>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Tirvest Advisors</t>
+          <t>Trivest Advisors</t>
         </is>
       </c>
       <c r="D61" t="inlineStr"/>
@@ -1935,7 +1935,7 @@
       <c r="B62" t="inlineStr"/>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Tirvest Advisors</t>
+          <t>Trivest Advisors</t>
         </is>
       </c>
       <c r="D62" t="inlineStr"/>

</xml_diff>